<commit_message>
racunice uz klizuci datum
</commit_message>
<xml_diff>
--- a/fenologija/NS_CE_AJ_2016.xlsx
+++ b/fenologija/NS_CE_AJ_2016.xlsx
@@ -1,25 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01_FAX\05_RADOVI\36_Poglavlje_Springer\CVETANJE\BBCH\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView windowWidth="28695" windowHeight="13080"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -47,28 +37,369 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="dd\.mm\.yyyy"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -76,33 +407,319 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -113,7 +730,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="4D4D4D"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -151,7 +768,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -186,7 +803,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -360,92 +977,86 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="8.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="1" max="1" width="10.14" style="1" customWidth="1"/>
+    <col min="2" max="5" width="8.42666666666667" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9.14" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:6">
+      <c r="A2" s="3">
         <v>42382</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <f>YEAR(A2)</f>
         <v>2016</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <f>MONTH(A2)</f>
         <v>1</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <f>DAY(A2)</f>
         <v>13</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <f>IF(C2=1,D2,IF(C2=2,D2+31,IF(C2=3,D2+31+29,IF(C2=4,D2+31+29+31,IF(C2=5,D2+31+29+31+30,IF(C2=6,D2+31+29+31+30+31,IF(C2=7,D2+31+29+31+30+31+30+31,D2+31+29+31+30+31+30+31+30)))))))</f>
         <v>13</v>
       </c>
       <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="3">
         <v>42408</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <f t="shared" ref="B3:B28" si="0">YEAR(A3)</f>
         <v>2016</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <f t="shared" ref="C3:C28" si="1">MONTH(A3)</f>
         <v>2</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <f t="shared" ref="D3:D28" si="2">DAY(A3)</f>
         <v>8</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <f t="shared" ref="E3:E28" si="3">IF(C3=1,D3,IF(C3=2,D3+31,IF(C3=3,D3+31+29,IF(C3=4,D3+31+29+31,IF(C3=5,D3+31+29+31+30,IF(C3=6,D3+31+29+31+30+31,IF(C3=7,D3+31+29+31+30+31+30+31,D3+31+29+31+30+31+30+31+30)))))))</f>
         <v>39</v>
       </c>
@@ -453,23 +1064,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="4" spans="1:6">
+      <c r="A4" s="3">
         <v>42417</v>
       </c>
-      <c r="B4" s="3">
-        <f t="shared" si="0"/>
-        <v>2016</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="B4" s="2">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="C4" s="2">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <f t="shared" si="3"/>
         <v>48</v>
       </c>
@@ -477,23 +1088,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="5" spans="1:6">
+      <c r="A5" s="3">
         <v>42423</v>
       </c>
-      <c r="B5" s="3">
-        <f t="shared" si="0"/>
-        <v>2016</v>
-      </c>
-      <c r="C5" s="3">
+      <c r="B5" s="2">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="C5" s="2">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <f t="shared" si="3"/>
         <v>54</v>
       </c>
@@ -501,23 +1112,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="6" spans="1:6">
+      <c r="A6" s="3">
         <v>42430</v>
       </c>
-      <c r="B6" s="3">
-        <f t="shared" si="0"/>
-        <v>2016</v>
-      </c>
-      <c r="C6" s="3">
+      <c r="B6" s="2">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="C6" s="2">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <f t="shared" si="3"/>
         <v>61</v>
       </c>
@@ -525,23 +1136,23 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="7" spans="1:6">
+      <c r="A7" s="3">
         <v>42437</v>
       </c>
-      <c r="B7" s="3">
-        <f t="shared" si="0"/>
-        <v>2016</v>
-      </c>
-      <c r="C7" s="3">
+      <c r="B7" s="2">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="C7" s="2">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <f t="shared" si="3"/>
         <v>68</v>
       </c>
@@ -549,23 +1160,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+    <row r="8" spans="1:6">
+      <c r="A8" s="3">
         <v>42444</v>
       </c>
-      <c r="B8" s="3">
-        <f t="shared" si="0"/>
-        <v>2016</v>
-      </c>
-      <c r="C8" s="3">
+      <c r="B8" s="2">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="C8" s="2">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <f t="shared" si="3"/>
         <v>75</v>
       </c>
@@ -573,23 +1184,23 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+    <row r="9" spans="1:6">
+      <c r="A9" s="3">
         <v>42451</v>
       </c>
-      <c r="B9" s="3">
-        <f t="shared" si="0"/>
-        <v>2016</v>
-      </c>
-      <c r="C9" s="3">
+      <c r="B9" s="2">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="C9" s="2">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <f t="shared" si="3"/>
         <v>82</v>
       </c>
@@ -597,23 +1208,23 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+    <row r="10" spans="1:6">
+      <c r="A10" s="3">
         <v>42458</v>
       </c>
-      <c r="B10" s="3">
-        <f t="shared" si="0"/>
-        <v>2016</v>
-      </c>
-      <c r="C10" s="3">
+      <c r="B10" s="2">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="C10" s="2">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <f t="shared" si="3"/>
         <v>89</v>
       </c>
@@ -621,23 +1232,23 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    <row r="11" spans="1:6">
+      <c r="A11" s="3">
         <v>42468</v>
       </c>
-      <c r="B11" s="3">
-        <f t="shared" si="0"/>
-        <v>2016</v>
-      </c>
-      <c r="C11" s="3">
+      <c r="B11" s="2">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="C11" s="2">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <f t="shared" si="3"/>
         <v>99</v>
       </c>
@@ -645,23 +1256,23 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+    <row r="12" spans="1:6">
+      <c r="A12" s="3">
         <v>42472</v>
       </c>
-      <c r="B12" s="3">
-        <f t="shared" si="0"/>
-        <v>2016</v>
-      </c>
-      <c r="C12" s="3">
+      <c r="B12" s="2">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="C12" s="2">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <f t="shared" si="3"/>
         <v>103</v>
       </c>
@@ -669,23 +1280,23 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+    <row r="13" spans="1:6">
+      <c r="A13" s="3">
         <v>42479</v>
       </c>
-      <c r="B13" s="3">
-        <f t="shared" si="0"/>
-        <v>2016</v>
-      </c>
-      <c r="C13" s="3">
+      <c r="B13" s="2">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="C13" s="2">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <f t="shared" si="3"/>
         <v>110</v>
       </c>
@@ -693,23 +1304,23 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+    <row r="14" spans="1:6">
+      <c r="A14" s="3">
         <v>42482</v>
       </c>
-      <c r="B14" s="3">
-        <f t="shared" si="0"/>
-        <v>2016</v>
-      </c>
-      <c r="C14" s="3">
+      <c r="B14" s="2">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="C14" s="2">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <f t="shared" si="3"/>
         <v>113</v>
       </c>
@@ -717,23 +1328,23 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+    <row r="15" spans="1:6">
+      <c r="A15" s="3">
         <v>42486</v>
       </c>
-      <c r="B15" s="3">
-        <f t="shared" si="0"/>
-        <v>2016</v>
-      </c>
-      <c r="C15" s="3">
+      <c r="B15" s="2">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="C15" s="2">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <f t="shared" si="3"/>
         <v>117</v>
       </c>
@@ -741,23 +1352,23 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+    <row r="16" spans="1:6">
+      <c r="A16" s="3">
         <v>42494</v>
       </c>
-      <c r="B16" s="3">
-        <f t="shared" si="0"/>
-        <v>2016</v>
-      </c>
-      <c r="C16" s="3">
+      <c r="B16" s="2">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="C16" s="2">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="2">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <f t="shared" si="3"/>
         <v>125</v>
       </c>
@@ -765,23 +1376,23 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+    <row r="17" spans="1:6">
+      <c r="A17" s="3">
         <v>42500</v>
       </c>
-      <c r="B17" s="3">
-        <f t="shared" si="0"/>
-        <v>2016</v>
-      </c>
-      <c r="C17" s="3">
+      <c r="B17" s="2">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="C17" s="2">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="2">
         <f t="shared" si="3"/>
         <v>131</v>
       </c>
@@ -789,23 +1400,23 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+    <row r="18" spans="1:6">
+      <c r="A18" s="3">
         <v>42507</v>
       </c>
-      <c r="B18" s="3">
-        <f t="shared" si="0"/>
-        <v>2016</v>
-      </c>
-      <c r="C18" s="3">
+      <c r="B18" s="2">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="C18" s="2">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="2">
         <f t="shared" si="3"/>
         <v>138</v>
       </c>
@@ -813,23 +1424,23 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+    <row r="19" spans="1:6">
+      <c r="A19" s="3">
         <v>42513</v>
       </c>
-      <c r="B19" s="3">
-        <f t="shared" si="0"/>
-        <v>2016</v>
-      </c>
-      <c r="C19" s="3">
+      <c r="B19" s="2">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="C19" s="2">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2">
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="2">
         <f t="shared" si="3"/>
         <v>144</v>
       </c>
@@ -837,23 +1448,23 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+    <row r="20" spans="1:6">
+      <c r="A20" s="3">
         <v>42520</v>
       </c>
-      <c r="B20" s="3">
-        <f t="shared" si="0"/>
-        <v>2016</v>
-      </c>
-      <c r="C20" s="3">
+      <c r="B20" s="2">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="C20" s="2">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <f t="shared" si="3"/>
         <v>151</v>
       </c>
@@ -861,23 +1472,23 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+    <row r="21" spans="1:6">
+      <c r="A21" s="3">
         <v>42527</v>
       </c>
-      <c r="B21" s="3">
-        <f t="shared" si="0"/>
-        <v>2016</v>
-      </c>
-      <c r="C21" s="3">
+      <c r="B21" s="2">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="C21" s="2">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="2">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <f t="shared" si="3"/>
         <v>158</v>
       </c>
@@ -885,23 +1496,23 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+    <row r="22" spans="1:6">
+      <c r="A22" s="3">
         <v>42534</v>
       </c>
-      <c r="B22" s="3">
-        <f t="shared" si="0"/>
-        <v>2016</v>
-      </c>
-      <c r="C22" s="3">
+      <c r="B22" s="2">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="C22" s="2">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="2">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <f t="shared" si="3"/>
         <v>165</v>
       </c>
@@ -909,23 +1520,23 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+    <row r="23" spans="1:6">
+      <c r="A23" s="3">
         <v>42542</v>
       </c>
-      <c r="B23" s="3">
-        <f t="shared" si="0"/>
-        <v>2016</v>
-      </c>
-      <c r="C23" s="3">
+      <c r="B23" s="2">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="C23" s="2">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="2">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <f t="shared" si="3"/>
         <v>173</v>
       </c>
@@ -933,23 +1544,23 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+    <row r="24" spans="1:6">
+      <c r="A24" s="3">
         <v>42544</v>
       </c>
-      <c r="B24" s="3">
-        <f t="shared" si="0"/>
-        <v>2016</v>
-      </c>
-      <c r="C24" s="3">
+      <c r="B24" s="2">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="C24" s="2">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="2">
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="2">
         <f t="shared" si="3"/>
         <v>175</v>
       </c>
@@ -957,23 +1568,23 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+    <row r="25" spans="1:6">
+      <c r="A25" s="3">
         <v>42548</v>
       </c>
-      <c r="B25" s="3">
-        <f t="shared" si="0"/>
-        <v>2016</v>
-      </c>
-      <c r="C25" s="3">
+      <c r="B25" s="2">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="C25" s="2">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="2">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="2">
         <f t="shared" si="3"/>
         <v>179</v>
       </c>
@@ -981,23 +1592,23 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+    <row r="26" spans="1:6">
+      <c r="A26" s="3">
         <v>42558</v>
       </c>
-      <c r="B26" s="3">
-        <f t="shared" si="0"/>
-        <v>2016</v>
-      </c>
-      <c r="C26" s="3">
+      <c r="B26" s="2">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="C26" s="2">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="2">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <f t="shared" si="3"/>
         <v>220</v>
       </c>
@@ -1005,23 +1616,23 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+    <row r="27" spans="1:6">
+      <c r="A27" s="3">
         <v>42572</v>
       </c>
-      <c r="B27" s="3">
-        <f t="shared" si="0"/>
-        <v>2016</v>
-      </c>
-      <c r="C27" s="3">
+      <c r="B27" s="2">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="C27" s="2">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="2">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="2">
         <f t="shared" si="3"/>
         <v>234</v>
       </c>
@@ -1029,23 +1640,23 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+    <row r="28" spans="1:6">
+      <c r="A28" s="3">
         <v>42583</v>
       </c>
-      <c r="B28" s="3">
-        <f t="shared" si="0"/>
-        <v>2016</v>
-      </c>
-      <c r="C28" s="3">
+      <c r="B28" s="2">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="C28" s="2">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="2">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="2">
         <f t="shared" si="3"/>
         <v>244</v>
       </c>
@@ -1055,5 +1666,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>